<commit_message>
EditProfileName Test Case Added
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\source\repos\mars.nunit-master\mars.nunit-master\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\source\repos\Sprint3.NUnit\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB924E8-DE12-4780-9889-71D40925D29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F712A22-6112-4274-B3B9-93D4DC0F2696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3970" yWindow="1110" windowWidth="13200" windowHeight="11060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="152">
   <si>
     <t>FirstName</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t>Save</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>Sheila Dimasuhid</t>
   </si>
 </sst>
 </file>
@@ -1127,99 +1133,120 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="20.08984375" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" customWidth="1"/>
-    <col min="5" max="5" width="24.81640625" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
-    <col min="10" max="10" width="52.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="20.08984375" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="24.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" customWidth="1"/>
+    <col min="13" max="13" width="52.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13">
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1232,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856D2F2D-9D6C-4FF9-93E3-CB98F3FE4A80}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
@@ -1339,11 +1366,11 @@
       </c>
       <c r="I2" s="8">
         <f ca="1">TODAY()+10</f>
-        <v>45071</v>
+        <v>45093</v>
       </c>
       <c r="J2" s="8">
         <f ca="1">TODAY()+20</f>
-        <v>45081</v>
+        <v>45103</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>62</v>
@@ -1398,11 +1425,11 @@
       </c>
       <c r="I3" s="8">
         <f t="shared" ref="I3:I8" ca="1" si="0">TODAY()+10</f>
-        <v>45071</v>
+        <v>45093</v>
       </c>
       <c r="J3" s="8">
         <f t="shared" ref="J3:J8" ca="1" si="1">TODAY()+20</f>
-        <v>45081</v>
+        <v>45103</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>62</v>
@@ -1459,11 +1486,11 @@
       </c>
       <c r="I4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45071</v>
+        <v>45093</v>
       </c>
       <c r="J4" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45081</v>
+        <v>45103</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>62</v>
@@ -1520,11 +1547,11 @@
       </c>
       <c r="I5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45071</v>
+        <v>45093</v>
       </c>
       <c r="J5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45081</v>
+        <v>45103</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>62</v>
@@ -1581,11 +1608,11 @@
       </c>
       <c r="I6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45071</v>
+        <v>45093</v>
       </c>
       <c r="J6" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45081</v>
+        <v>45103</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>62</v>
@@ -1651,11 +1678,11 @@
       </c>
       <c r="I8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45071</v>
+        <v>45093</v>
       </c>
       <c r="J8" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45081</v>
+        <v>45103</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Added Test cases for Full Name, Availability, Hours, Earn Target. Started implementing Description test case.
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\source\repos\Sprint3.NUnit\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F712A22-6112-4274-B3B9-93D4DC0F2696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57AAAD1-CFB0-4837-9A59-3EBC16768A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22545" yWindow="5025" windowWidth="19485" windowHeight="9210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="160">
   <si>
     <t>FirstName</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Full time</t>
-  </si>
-  <si>
     <t>New Zealand</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>4 years as Manual Tester and 3 Years as Automation Tester</t>
   </si>
   <si>
-    <t>fgh</t>
-  </si>
-  <si>
     <t>jkl</t>
   </si>
   <si>
@@ -510,6 +504,36 @@
   </si>
   <si>
     <t>Sheila Dimasuhid</t>
+  </si>
+  <si>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>AvailableHours</t>
+  </si>
+  <si>
+    <t>Less than 30hours a week</t>
+  </si>
+  <si>
+    <t>More than 30hours a week</t>
+  </si>
+  <si>
+    <t>As needed</t>
+  </si>
+  <si>
+    <t>Part Time</t>
+  </si>
+  <si>
+    <t>Less than $500 per month</t>
+  </si>
+  <si>
+    <t>EarnTarget</t>
+  </si>
+  <si>
+    <t>Between $500 and $1000 per month</t>
+  </si>
+  <si>
+    <t>More than $1000 per month</t>
   </si>
 </sst>
 </file>
@@ -520,12 +544,33 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -600,40 +645,43 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1049,19 +1097,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1103,13 +1151,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1133,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1144,17 +1192,20 @@
     <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="20.08984375" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" customWidth="1"/>
-    <col min="8" max="8" width="24.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" customWidth="1"/>
-    <col min="12" max="12" width="18.453125" customWidth="1"/>
-    <col min="13" max="13" width="52.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.08984375" customWidth="1"/>
+    <col min="9" max="9" width="18.26953125" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" customWidth="1"/>
+    <col min="15" max="15" width="52.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1162,96 +1213,123 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+    </row>
+    <row r="3" spans="1:15">
+      <c r="D3" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="D3" t="s">
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="E4" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1284,96 +1362,96 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="P1" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="D2" s="7" t="str">
         <f>IFERROR(LEFT(C2,FIND(" ",C2)-1),C2)</f>
         <v>Programming</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="H2" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I2" s="8">
         <f ca="1">TODAY()+10</f>
-        <v>45093</v>
+        <v>45100</v>
       </c>
       <c r="J2" s="8">
         <f ca="1">TODAY()+20</f>
-        <v>45103</v>
+        <v>45110</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L2" s="10">
         <v>0.75</v>
@@ -1382,7 +1460,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O2" s="5" t="str">
         <f>IF(N2=[1]Data!$B$18,"Programming","")</f>
@@ -1393,46 +1471,46 @@
         <v>9</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="7" t="str">
         <f>IFERROR(LEFT(C3,FIND(" ",C3)-1),C3)</f>
         <v>Programming</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="H3" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I3" s="8">
         <f t="shared" ref="I3:I8" ca="1" si="0">TODAY()+10</f>
-        <v>45093</v>
+        <v>45100</v>
       </c>
       <c r="J3" s="8">
         <f t="shared" ref="J3:J8" ca="1" si="1">TODAY()+20</f>
-        <v>45103</v>
+        <v>45110</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L3" s="10">
         <v>0.75</v>
@@ -1441,7 +1519,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O3" s="5" t="str">
         <f>IF(N3=[1]Data!$B$18,"Programming","")</f>
@@ -1452,48 +1530,48 @@
         <v>9</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="7" t="str">
         <f>IFERROR(LEFT(C4,FIND(" ",C4)-1),C4)</f>
         <v>Programming</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="H4" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45093</v>
+        <v>45100</v>
       </c>
       <c r="J4" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45103</v>
+        <v>45110</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L4" s="10">
         <v>0.75</v>
@@ -1502,7 +1580,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O4" s="5" t="str">
         <f>IF(N4=[1]Data!$B$18,"Programming","")</f>
@@ -1513,48 +1591,48 @@
         <v>9</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="D5" s="7" t="str">
         <f>IFERROR(LEFT(C5,FIND(" ",C5)-1),C5)</f>
         <v>Programming</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="H5" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45093</v>
+        <v>45100</v>
       </c>
       <c r="J5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45103</v>
+        <v>45110</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L5" s="10">
         <v>0.75</v>
@@ -1563,7 +1641,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O5" s="5" t="str">
         <f>IF(N5=[1]Data!$B$18,"Programming","")</f>
@@ -1574,48 +1652,48 @@
         <v>9</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="7" t="str">
         <f>IFERROR(LEFT(C6,FIND(" ",C6)-1),C6)</f>
         <v>Programming</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="H6" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45093</v>
+        <v>45100</v>
       </c>
       <c r="J6" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45103</v>
+        <v>45110</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L6" s="10">
         <v>0.75</v>
@@ -1624,7 +1702,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O6" s="5" t="str">
         <f>IF(N6=[1]Data!$B$18,"Programming","")</f>
@@ -1635,10 +1713,10 @@
         <v>9</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -1652,40 +1730,40 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" s="7" t="str">
         <f>IFERROR(LEFT(C8,FIND(" ",C8)-1),C8)</f>
         <v>Programming</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45093</v>
+        <v>45100</v>
       </c>
       <c r="J8" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45103</v>
+        <v>45110</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L8" s="10">
         <v>0.75</v>
@@ -1694,7 +1772,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O8" s="5" t="str">
         <f>IF(N8=[1]Data!$B$18,"Programming","")</f>
@@ -1705,10 +1783,10 @@
         <v/>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1750,44 +1828,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
-      <c r="A2" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="16"/>
+      <c r="A2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="18"/>
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="J3" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1795,34 +1873,34 @@
         <v>1</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="H4" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1830,34 +1908,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="G5" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="I5" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="J5" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="K5" s="15" t="s">
         <v>106</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1865,34 +1943,34 @@
         <v>3</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="E6" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="F6" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="G6" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="H6" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="I6" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="J6" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="K6" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1900,34 +1978,34 @@
         <v>4</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="E7" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="F7" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="G7" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="H7" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="K7" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1935,28 +2013,28 @@
         <v>5</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="E8" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="J8" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="K8" s="15" t="s">
         <v>131</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1964,19 +2042,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1984,10 +2062,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1995,73 +2073,73 @@
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D11" s="12"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2097,10 +2175,10 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2120,10 +2198,10 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -2163,75 +2241,75 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>48</v>
       </c>
-      <c r="H2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2">
         <v>10</v>

</xml_diff>

<commit_message>
Added Profile Description Test cases - on progress
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\source\repos\Sprint3.NUnit\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57AAAD1-CFB0-4837-9A59-3EBC16768A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED79073-3E84-40DD-A5A8-6F0415C1E736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22545" yWindow="5025" windowWidth="19485" windowHeight="9210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27075" yWindow="4785" windowWidth="18030" windowHeight="10320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="165">
   <si>
     <t>FirstName</t>
   </si>
@@ -534,6 +534,63 @@
   </si>
   <si>
     <t>More than $1000 per month</t>
+  </si>
+  <si>
+    <t>I love coding and working on my skill to improve and get better to become a Software Tester.</t>
+  </si>
+  <si>
+    <t>This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+This is another test to check if description will accept more than 598 characters.
+A total of 597 characters including spaces and periods.</t>
+  </si>
+  <si>
+    <t>Invalid characters</t>
+  </si>
+  <si>
+    <t>Empty description</t>
+  </si>
+  <si>
+    <t>description starts with a space followed by a valid description</t>
   </si>
 </sst>
 </file>
@@ -544,12 +601,26 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -645,43 +716,46 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1181,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1195,17 +1269,18 @@
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
     <col min="5" max="5" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.08984375" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" customWidth="1"/>
-    <col min="10" max="10" width="24.81640625" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
-    <col min="14" max="14" width="18.453125" customWidth="1"/>
-    <col min="15" max="15" width="52.7265625" customWidth="1"/>
+    <col min="7" max="7" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.08984375" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="18.453125" customWidth="1"/>
+    <col min="16" max="16" width="52.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1224,35 +1299,38 @@
       <c r="F1" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1268,63 +1346,82 @@
       <c r="E2" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="D3" s="16" t="s">
         <v>155</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="G3" t="s">
-        <v>26</v>
+      <c r="G3" s="22" t="s">
+        <v>161</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
       <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="E4" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>159</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="G5" s="21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="G6" s="21" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1444,11 +1541,11 @@
       </c>
       <c r="I2" s="8">
         <f ca="1">TODAY()+10</f>
-        <v>45100</v>
+        <v>45102</v>
       </c>
       <c r="J2" s="8">
         <f ca="1">TODAY()+20</f>
-        <v>45110</v>
+        <v>45112</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>60</v>
@@ -1503,11 +1600,11 @@
       </c>
       <c r="I3" s="8">
         <f t="shared" ref="I3:I8" ca="1" si="0">TODAY()+10</f>
-        <v>45100</v>
+        <v>45102</v>
       </c>
       <c r="J3" s="8">
         <f t="shared" ref="J3:J8" ca="1" si="1">TODAY()+20</f>
-        <v>45110</v>
+        <v>45112</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>60</v>
@@ -1564,11 +1661,11 @@
       </c>
       <c r="I4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45100</v>
+        <v>45102</v>
       </c>
       <c r="J4" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45110</v>
+        <v>45112</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>60</v>
@@ -1625,11 +1722,11 @@
       </c>
       <c r="I5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45100</v>
+        <v>45102</v>
       </c>
       <c r="J5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45110</v>
+        <v>45112</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>60</v>
@@ -1686,11 +1783,11 @@
       </c>
       <c r="I6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45100</v>
+        <v>45102</v>
       </c>
       <c r="J6" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45110</v>
+        <v>45112</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>60</v>
@@ -1756,11 +1853,11 @@
       </c>
       <c r="I8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45100</v>
+        <v>45102</v>
       </c>
       <c r="J8" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45110</v>
+        <v>45112</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>60</v>
@@ -1828,10 +1925,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
     </row>

</xml_diff>

<commit_message>
Added 7 test cases for Profile Description. 5 Test cases involves Invalid inputs.
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\source\repos\Sprint3.NUnit\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED79073-3E84-40DD-A5A8-6F0415C1E736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD265AE4-ED69-4D7E-93DF-9AFF144CC39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27075" yWindow="4785" windowWidth="18030" windowHeight="10320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -539,58 +539,19 @@
     <t>I love coding and working on my skill to improve and get better to become a Software Tester.</t>
   </si>
   <si>
-    <t>This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-This is another test to check if description will accept more than 598 characters.
-A total of 597 characters including spaces and periods.</t>
-  </si>
-  <si>
-    <t>Invalid characters</t>
-  </si>
-  <si>
-    <t>Empty description</t>
-  </si>
-  <si>
-    <t>description starts with a space followed by a valid description</t>
+    <t xml:space="preserve">This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters.
+This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters. This is another test to check if description will accept more than 600 characters.
+</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;*()_+&lt;&gt;,.?~`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This description starts with a space.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heaps of unwanted spaces after a valid text. Total of 236 characters.
+</t>
   </si>
 </sst>
 </file>
@@ -601,12 +562,19 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -716,46 +684,47 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1257,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1269,7 +1238,7 @@
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
     <col min="5" max="5" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.81640625" customWidth="1"/>
     <col min="8" max="9" width="20.08984375" customWidth="1"/>
     <col min="10" max="10" width="18.26953125" customWidth="1"/>
     <col min="11" max="11" width="24.81640625" customWidth="1"/>
@@ -1390,7 +1359,7 @@
       <c r="F3" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>161</v>
       </c>
       <c r="H3" t="s">
@@ -1410,17 +1379,17 @@
       <c r="F4" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1541,11 +1510,11 @@
       </c>
       <c r="I2" s="8">
         <f ca="1">TODAY()+10</f>
-        <v>45102</v>
+        <v>45105</v>
       </c>
       <c r="J2" s="8">
         <f ca="1">TODAY()+20</f>
-        <v>45112</v>
+        <v>45115</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>60</v>
@@ -1600,11 +1569,11 @@
       </c>
       <c r="I3" s="8">
         <f t="shared" ref="I3:I8" ca="1" si="0">TODAY()+10</f>
-        <v>45102</v>
+        <v>45105</v>
       </c>
       <c r="J3" s="8">
         <f t="shared" ref="J3:J8" ca="1" si="1">TODAY()+20</f>
-        <v>45112</v>
+        <v>45115</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>60</v>
@@ -1661,11 +1630,11 @@
       </c>
       <c r="I4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45102</v>
+        <v>45105</v>
       </c>
       <c r="J4" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45112</v>
+        <v>45115</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>60</v>
@@ -1722,11 +1691,11 @@
       </c>
       <c r="I5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45102</v>
+        <v>45105</v>
       </c>
       <c r="J5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45112</v>
+        <v>45115</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>60</v>
@@ -1783,11 +1752,11 @@
       </c>
       <c r="I6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45102</v>
+        <v>45105</v>
       </c>
       <c r="J6" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45112</v>
+        <v>45115</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>60</v>
@@ -1853,11 +1822,11 @@
       </c>
       <c r="I8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45102</v>
+        <v>45105</v>
       </c>
       <c r="J8" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>45112</v>
+        <v>45115</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>60</v>
@@ -1925,10 +1894,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
     </row>

</xml_diff>